<commit_message>
changed ais to 1 - 3 scale
</commit_message>
<xml_diff>
--- a/data/ais_effects.xlsx
+++ b/data/ais_effects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bcgov-my.sharepoint.com/personal/john_phelan_gov_bc_ca/Documents/R_projects/SAR_prioritization_model/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="8_{5875F5B9-1EFB-4B19-A375-CA6D5AB4B6C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E376395D-13F4-4892-980A-A062FD05787E}"/>
+  <xr:revisionPtr revIDLastSave="134" documentId="8_{5875F5B9-1EFB-4B19-A375-CA6D5AB4B6C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7E3B20D-BAF5-45C8-8C0A-146D7DD34B55}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CBBAE9E4-278C-472C-BDAB-08A259D82961}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
   <si>
     <t>Species</t>
   </si>
@@ -90,7 +90,31 @@
     <t>Black Bullhead</t>
   </si>
   <si>
-    <t>Black bullead</t>
+    <t>Channel Catfish</t>
+  </si>
+  <si>
+    <t>Common Carp</t>
+  </si>
+  <si>
+    <t>Black Bullead</t>
+  </si>
+  <si>
+    <t>Largemouth Bass</t>
+  </si>
+  <si>
+    <t>Pumpkinseed</t>
+  </si>
+  <si>
+    <t>Tench</t>
+  </si>
+  <si>
+    <t>Smallmouth Bass</t>
+  </si>
+  <si>
+    <t>Yellow Perch</t>
+  </si>
+  <si>
+    <t>Walleye</t>
   </si>
 </sst>
 </file>
@@ -157,6 +181,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -476,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFDDCAB6-DA5F-4600-A8A2-36CFF1995E09}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,16 +548,16 @@
         <v>1</v>
       </c>
       <c r="C2" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" s="1">
         <v>2</v>
       </c>
       <c r="E2" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F2" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -540,7 +568,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
@@ -549,7 +577,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -560,16 +588,16 @@
         <v>1</v>
       </c>
       <c r="C4" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
       </c>
       <c r="F4" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -577,19 +605,19 @@
         <v>9</v>
       </c>
       <c r="B5" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E5" s="1">
         <v>2</v>
       </c>
       <c r="F5" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -600,36 +628,36 @@
         <v>1</v>
       </c>
       <c r="C6" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D6" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E6" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F6" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C7" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D7" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E7" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -637,19 +665,167 @@
         <v>16</v>
       </c>
       <c r="B8" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D8" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E8" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8" s="1">
-        <v>3</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="1">
+        <v>3</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="1">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1">
+        <v>3</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="1">
+        <v>3</v>
+      </c>
+      <c r="C11" s="1">
+        <v>2</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1">
+        <v>1</v>
+      </c>
+      <c r="F11" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="1">
+        <v>2</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="1">
+        <v>2</v>
+      </c>
+      <c r="C13" s="1">
+        <v>2</v>
+      </c>
+      <c r="D13" s="1">
+        <v>3</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="1">
+        <v>3</v>
+      </c>
+      <c r="C14" s="1">
+        <v>3</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="1">
+        <v>3</v>
+      </c>
+      <c r="C16" s="1">
+        <v>3</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -659,10 +835,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF761907-985C-41A7-8BDE-F49BAD096099}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -695,7 +871,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -703,19 +879,19 @@
         <v>1</v>
       </c>
       <c r="C2" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F2" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -723,7 +899,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
@@ -732,10 +908,10 @@
         <v>1</v>
       </c>
       <c r="F3" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -743,7 +919,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" s="1">
         <v>1</v>
@@ -752,7 +928,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -760,22 +936,22 @@
         <v>13</v>
       </c>
       <c r="B5" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D5" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E5" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
@@ -783,55 +959,95 @@
         <v>1</v>
       </c>
       <c r="C6" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D6" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E6" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F6" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C7" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D7" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E7" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="1">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="1">
-        <v>4</v>
-      </c>
-      <c r="C8" s="1">
-        <v>2</v>
-      </c>
-      <c r="D8" s="1">
-        <v>4</v>
-      </c>
-      <c r="E8" s="1">
-        <v>1</v>
-      </c>
-      <c r="F8" s="1">
+      <c r="B9" s="1">
+        <v>3</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1">
+        <v>3</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
time capsule from just before splitting SARA into separate rows
</commit_message>
<xml_diff>
--- a/data/ais_effects.xlsx
+++ b/data/ais_effects.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bcgov-my.sharepoint.com/personal/john_phelan_gov_bc_ca/Documents/R_projects/SAR_prioritization_model/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CMADSEN\Downloads\LocalR\long_term_projects\SAR_prioritization_model\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="266" documentId="8_{5875F5B9-1EFB-4B19-A375-CA6D5AB4B6C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D3395C05-2546-47C6-889E-B495339C3144}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8166A717-0EAB-4366-B371-E739C6A6689D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CBBAE9E4-278C-472C-BDAB-08A259D82961}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{CBBAE9E4-278C-472C-BDAB-08A259D82961}"/>
   </bookViews>
   <sheets>
     <sheet name="fish" sheetId="1" r:id="rId1"/>
@@ -63,9 +63,6 @@
     <t xml:space="preserve">Chinese Mystery Snail </t>
   </si>
   <si>
-    <t>Rosy Redhead Fathead Minnow</t>
-  </si>
-  <si>
     <t xml:space="preserve">Goldfish </t>
   </si>
   <si>
@@ -145,6 +142,9 @@
   </si>
   <si>
     <t>Yellow Bullead</t>
+  </si>
+  <si>
+    <t>Rosy Red Fathead Minnow</t>
   </si>
 </sst>
 </file>
@@ -211,10 +211,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -536,22 +532,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFDDCAB6-DA5F-4600-A8A2-36CFF1995E09}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -571,10 +567,10 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -597,7 +593,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -620,32 +616,32 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1">
-        <v>3</v>
-      </c>
-      <c r="D4" s="1">
-        <v>1</v>
-      </c>
-      <c r="E4" s="1">
-        <v>1</v>
-      </c>
-      <c r="F4" s="1">
-        <v>2</v>
-      </c>
-      <c r="G4" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="B5" s="1">
         <v>2</v>
@@ -664,32 +660,32 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1">
+        <v>2</v>
+      </c>
+      <c r="F6" s="1">
+        <v>2</v>
+      </c>
+      <c r="G6" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="B6" s="1">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1">
-        <v>2</v>
-      </c>
-      <c r="D6" s="1">
-        <v>2</v>
-      </c>
-      <c r="E6" s="1">
-        <v>2</v>
-      </c>
-      <c r="F6" s="1">
-        <v>2</v>
-      </c>
-      <c r="G6" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1">
@@ -706,9 +702,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="1">
         <v>3</v>
@@ -727,9 +723,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" s="1">
         <v>3</v>
@@ -748,9 +744,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B10" s="1">
         <v>3</v>
@@ -769,9 +765,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" s="1">
         <v>3</v>
@@ -788,9 +784,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" s="1">
         <v>3</v>
@@ -807,9 +803,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" s="1">
         <v>3</v>
@@ -826,9 +822,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" s="1">
         <v>2</v>
@@ -843,9 +839,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" s="1">
         <v>2</v>
@@ -864,9 +860,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16" s="1">
         <v>3</v>
@@ -883,20 +879,20 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="1">
+        <v>2</v>
+      </c>
+      <c r="G17" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="C17" s="1">
-        <v>2</v>
-      </c>
-      <c r="G17" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="B18" s="1">
         <v>3</v>
@@ -911,9 +907,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B19" s="1">
         <v>2</v>
@@ -925,51 +921,51 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="1">
+        <v>3</v>
+      </c>
+      <c r="F20">
+        <v>2</v>
+      </c>
+      <c r="G20" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="1">
-        <v>3</v>
-      </c>
-      <c r="F20">
-        <v>2</v>
-      </c>
-      <c r="G20" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="C21" s="1">
+        <v>3</v>
+      </c>
+      <c r="G21" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="1">
-        <v>3</v>
-      </c>
-      <c r="G21" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22" s="1">
+        <v>3</v>
+      </c>
+      <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="G22" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="B22">
-        <v>2</v>
-      </c>
-      <c r="C22" s="1">
-        <v>3</v>
-      </c>
-      <c r="D22">
-        <v>3</v>
-      </c>
-      <c r="G22" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -999,21 +995,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF761907-985C-41A7-8BDE-F49BAD096099}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1033,10 +1029,10 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1055,9 +1051,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -1074,9 +1070,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1087,9 +1083,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1">
@@ -1104,32 +1100,32 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1">
+        <v>2</v>
+      </c>
+      <c r="F6" s="1">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="B6" s="1">
-        <v>2</v>
-      </c>
-      <c r="C6" s="1">
-        <v>2</v>
-      </c>
-      <c r="D6" s="1">
-        <v>2</v>
-      </c>
-      <c r="E6" s="1">
-        <v>2</v>
-      </c>
-      <c r="F6" s="1">
-        <v>2</v>
-      </c>
-      <c r="G6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="B7" s="1">
         <v>3</v>
@@ -1148,9 +1144,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1">
         <v>3</v>
@@ -1163,9 +1159,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B9" s="1">
         <v>3</v>
@@ -1178,9 +1174,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B10" s="1">
         <v>3</v>
@@ -1193,9 +1189,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" s="1">
         <v>2</v>
@@ -1208,9 +1204,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1223,9 +1219,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1236,9 +1232,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" s="1">
         <v>2</v>
@@ -1251,9 +1247,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" s="1">
         <v>3</v>
@@ -1268,9 +1264,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16" s="1">
         <v>1</v>
@@ -1283,18 +1279,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C17" s="1"/>
       <c r="G17">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1305,44 +1301,44 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G19">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G20">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="G21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G21">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="G22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="D22">
-        <v>2</v>
-      </c>
-      <c r="G22">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="D23">
         <v>3</v>

</xml_diff>